<commit_message>
Stock item in excel
</commit_message>
<xml_diff>
--- a/ExcelFiles/StockDomain.xlsx
+++ b/ExcelFiles/StockDomain.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Cellma4Automation\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09D117E-F203-463A-BE06-A2C11D5FDB18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99C429E-5333-4CD4-B5D2-17EBAB1090FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3240" yWindow="3240" windowWidth="18000" windowHeight="9270" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -299,7 +299,7 @@
     <t>8</t>
   </si>
   <si>
-    <t>Dcold</t>
+    <t>DcoldA</t>
   </si>
 </sst>
 </file>
@@ -1021,7 +1021,7 @@
     <row r="2" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="str">
         <f>AddNewStock!A2</f>
-        <v>Dcold</v>
+        <v>DcoldA</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Stock Item Change in excel
</commit_message>
<xml_diff>
--- a/ExcelFiles/StockDomain.xlsx
+++ b/ExcelFiles/StockDomain.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Cellma4Automation\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE0FEA3-9AAF-4669-9450-151342C378A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92DE5641-9A2B-4CE4-91D3-F23DFD7303B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="1" r:id="rId1"/>
@@ -299,7 +299,7 @@
     <t>8</t>
   </si>
   <si>
-    <t>Vicks150</t>
+    <t>IBU Profen</t>
   </si>
 </sst>
 </file>
@@ -664,7 +664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -746,7 +746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6834B6FC-CAD9-422A-8F3B-C1D76C190C8D}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1021,7 +1021,7 @@
     <row r="2" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="str">
         <f>AddNewStock!A2</f>
-        <v>Vicks150</v>
+        <v>IBU Profen</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>

</xml_diff>